<commit_message>
Final update with issues numbers in CV32E40Pv2 waiver list file.
Signed-off-by: Pascal Gouedo <pascal.gouedo@dolphin.fr>
</commit_message>
<xml_diff>
--- a/Project-Descriptions-and-Plans/CV32E40Pv2/Milestone-data/RTL_v1.8.3/CV32E40Pv2_waiver_list.xlsx
+++ b/Project-Descriptions-and-Plans/CV32E40Pv2/Milestone-data/RTL_v1.8.3/CV32E40Pv2_waiver_list.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\core-v-docs\Project-Descriptions-and-Plans\CV32E40Pv2\Milestone-data\RTL_v1.8.0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\core-v-docs\Project-Descriptions-and-Plans\CV32E40Pv2\Milestone-data\RTL_v1.8.3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8653A3BB-594A-43F9-82F9-1818841C0638}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF55ECBA-A416-49F6-ADEC-8BD80B77925D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="774" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
     <sheet name="func_cov (debug)" sheetId="8" r:id="rId7"/>
     <sheet name="func_cov (hwloop)" sheetId="10" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="191028" iterateDelta="1E-4"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2312" uniqueCount="314">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2312" uniqueCount="315">
   <si>
     <t>code cov waiver</t>
   </si>
@@ -886,9 +886,6 @@
   </si>
   <si>
     <t>feccondrow 872 5</t>
-  </si>
-  <si>
-    <t>&lt;to file ticket&gt;</t>
   </si>
   <si>
     <t>Specific combination is unreachable. Proven with Formal</t>
@@ -986,6 +983,19 @@
   <si>
     <t>#1006
 #1007</t>
+  </si>
+  <si>
+    <t>#1022</t>
+  </si>
+  <si>
+    <t>#1011
+#1012
+#1015
+#1016
+#1017
+#1018
+#1019
+#1023</t>
   </si>
 </sst>
 </file>
@@ -1601,7 +1611,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1638,7 +1648,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1666,10 +1675,6 @@
     </xf>
     <xf numFmtId="0" fontId="19" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -2542,9 +2547,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D84"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K29" sqref="K29"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2556,16 +2559,16 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="19"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="18"/>
     </row>
     <row r="3" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>129</v>
@@ -2857,7 +2860,6 @@
       </c>
     </row>
     <row r="31" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A31" s="25"/>
       <c r="B31">
         <v>28</v>
       </c>
@@ -2869,7 +2871,6 @@
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="25"/>
       <c r="B32">
         <v>29</v>
       </c>
@@ -2881,8 +2882,8 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="25" t="s">
-        <v>311</v>
+      <c r="A33" t="s">
+        <v>310</v>
       </c>
       <c r="B33">
         <v>30</v>
@@ -2895,8 +2896,8 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" s="25" t="s">
-        <v>312</v>
+      <c r="A34" t="s">
+        <v>311</v>
       </c>
       <c r="B34">
         <v>31</v>
@@ -2909,21 +2910,20 @@
       </c>
     </row>
     <row r="35" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A35" s="26" t="s">
-        <v>313</v>
+      <c r="A35" s="1" t="s">
+        <v>312</v>
       </c>
       <c r="B35">
         <v>32</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D35" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" s="25"/>
       <c r="B36">
         <v>33</v>
       </c>
@@ -2935,7 +2935,6 @@
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37" s="25"/>
       <c r="B37">
         <v>34</v>
       </c>
@@ -2947,7 +2946,6 @@
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A38" s="25"/>
       <c r="B38">
         <v>35</v>
       </c>
@@ -2959,7 +2957,6 @@
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" s="25"/>
       <c r="B39">
         <v>36</v>
       </c>
@@ -2971,7 +2968,6 @@
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40" s="25"/>
       <c r="B40">
         <v>37</v>
       </c>
@@ -3169,15 +3165,15 @@
         <v>125</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A58" s="14" t="s">
-        <v>281</v>
+    <row r="58" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A58" s="1" t="s">
+        <v>314</v>
       </c>
       <c r="B58">
         <v>55</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D58" t="s">
         <v>125</v>
@@ -3261,8 +3257,8 @@
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A66" s="14" t="s">
-        <v>281</v>
+      <c r="A66" t="s">
+        <v>313</v>
       </c>
       <c r="B66">
         <v>63</v>
@@ -3290,7 +3286,7 @@
         <v>65</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D68" t="s">
         <v>125</v>
@@ -3301,7 +3297,7 @@
         <v>66</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D69" t="s">
         <v>125</v>
@@ -3312,7 +3308,7 @@
         <v>67</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D70" t="s">
         <v>125</v>
@@ -3323,7 +3319,7 @@
         <v>68</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D71" t="s">
         <v>125</v>
@@ -3334,7 +3330,7 @@
         <v>69</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D72" t="s">
         <v>125</v>
@@ -3345,7 +3341,7 @@
         <v>70</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D73" t="s">
         <v>125</v>
@@ -3356,7 +3352,7 @@
         <v>71</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D74" t="s">
         <v>125</v>
@@ -3364,12 +3360,12 @@
     </row>
     <row r="77" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="78" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A78" s="17" t="s">
+      <c r="A78" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="B78" s="18"/>
-      <c r="C78" s="18"/>
-      <c r="D78" s="19"/>
+      <c r="B78" s="17"/>
+      <c r="C78" s="17"/>
+      <c r="D78" s="18"/>
     </row>
     <row r="79" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
@@ -3459,7 +3455,7 @@
   <dimension ref="A1:F172"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B175" sqref="B175"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3473,14 +3469,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="19" t="s">
         <v>126</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
     </row>
     <row r="2" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
@@ -6334,7 +6330,7 @@
         <v>57</v>
       </c>
       <c r="D166" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E166" s="3" t="s">
         <v>46</v>
@@ -6354,7 +6350,7 @@
         <v>57</v>
       </c>
       <c r="D167" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E167" s="3" t="s">
         <v>46</v>
@@ -6374,7 +6370,7 @@
         <v>57</v>
       </c>
       <c r="D168" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E168" s="3" t="s">
         <v>46</v>
@@ -6394,7 +6390,7 @@
         <v>57</v>
       </c>
       <c r="D169" s="3" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E169" s="3" t="s">
         <v>46</v>
@@ -6414,7 +6410,7 @@
         <v>57</v>
       </c>
       <c r="D170" s="3" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E170" s="3" t="s">
         <v>46</v>
@@ -6434,10 +6430,10 @@
         <v>57</v>
       </c>
       <c r="D171" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="E171" s="3" t="s">
         <v>307</v>
-      </c>
-      <c r="E171" s="3" t="s">
-        <v>308</v>
       </c>
       <c r="F171" s="3">
         <v>55</v>
@@ -6457,7 +6453,7 @@
         <v>59</v>
       </c>
       <c r="E172" s="3" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F172" s="3">
         <v>17</v>
@@ -6493,14 +6489,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="20" t="s">
         <v>127</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="22"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="21"/>
     </row>
     <row r="2" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
@@ -6835,7 +6831,7 @@
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="15">
+      <c r="A21" s="14">
         <v>241</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -6852,7 +6848,7 @@
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" s="15">
+      <c r="A22" s="14">
         <v>529</v>
       </c>
       <c r="B22" s="1" t="s">
@@ -6869,7 +6865,7 @@
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" s="15">
+      <c r="A23" s="14">
         <v>1558</v>
       </c>
       <c r="B23" s="1" t="s">
@@ -6886,7 +6882,7 @@
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" s="15">
+      <c r="A24" s="14">
         <v>1559</v>
       </c>
       <c r="B24" s="1" t="s">
@@ -6903,7 +6899,7 @@
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" s="15">
+      <c r="A25" s="14">
         <v>1560</v>
       </c>
       <c r="B25" s="1" t="s">
@@ -6920,7 +6916,7 @@
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" s="15">
+      <c r="A26" s="14">
         <v>1561</v>
       </c>
       <c r="B26" s="1" t="s">
@@ -6937,7 +6933,7 @@
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A27" s="15">
+      <c r="A27" s="14">
         <v>1562</v>
       </c>
       <c r="B27" s="1" t="s">
@@ -6954,7 +6950,7 @@
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A28" s="15">
+      <c r="A28" s="14">
         <v>529</v>
       </c>
       <c r="B28" s="1" t="s">
@@ -6971,7 +6967,7 @@
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A29" s="15">
+      <c r="A29" s="14">
         <v>1557</v>
       </c>
       <c r="B29" s="1" t="s">
@@ -6988,7 +6984,7 @@
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A30" s="15">
+      <c r="A30" s="14">
         <v>236</v>
       </c>
       <c r="B30" s="1" t="s">
@@ -7005,7 +7001,7 @@
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A31" s="15">
+      <c r="A31" s="14">
         <v>242</v>
       </c>
       <c r="B31" s="1" t="s">
@@ -7022,7 +7018,7 @@
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A32" s="15">
+      <c r="A32" s="14">
         <v>248</v>
       </c>
       <c r="B32" s="1" t="s">
@@ -7462,7 +7458,7 @@
   <dimension ref="A1:F398"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D245" sqref="D245"/>
+      <selection activeCell="F360" sqref="F360"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7476,14 +7472,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="20" t="s">
         <v>128</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="22"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="21"/>
     </row>
     <row r="2" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
@@ -7506,7 +7502,7 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="15">
+      <c r="A3" s="14">
         <v>1264</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -7523,7 +7519,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="15">
+      <c r="A4" s="14">
         <v>1265</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -7540,7 +7536,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="15">
+      <c r="A5" s="14">
         <v>1266</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -7557,7 +7553,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="15">
+      <c r="A6" s="14">
         <v>1273</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -7574,7 +7570,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="15">
+      <c r="A7" s="14">
         <v>1274</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -7591,7 +7587,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="15">
+      <c r="A8" s="14">
         <v>1275</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -7608,7 +7604,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="15">
+      <c r="A9" s="14">
         <v>1295</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -7625,7 +7621,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="15">
+      <c r="A10" s="14">
         <v>1296</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -7642,7 +7638,7 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="15">
+      <c r="A11" s="14">
         <v>1297</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -7659,7 +7655,7 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="15">
+      <c r="A12" s="14">
         <v>1353</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -7676,7 +7672,7 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="15">
+      <c r="A13" s="14">
         <v>1362</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -7693,7 +7689,7 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="15">
+      <c r="A14" s="14">
         <v>1440</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -7710,7 +7706,7 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="15">
+      <c r="A15" s="14">
         <v>1483</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -7727,7 +7723,7 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="16">
+      <c r="A16" s="15">
         <v>201</v>
       </c>
       <c r="B16" t="s">
@@ -7745,7 +7741,7 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="16">
+      <c r="A17" s="15">
         <v>202</v>
       </c>
       <c r="B17" t="s">
@@ -8085,7 +8081,7 @@
         <v>149</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F35" s="1">
         <v>55</v>
@@ -8102,7 +8098,7 @@
         <v>149</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F36" s="1">
         <v>55</v>
@@ -8119,7 +8115,7 @@
         <v>149</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F37" s="1">
         <v>55</v>
@@ -8139,7 +8135,7 @@
         <v>228</v>
       </c>
       <c r="E38" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="F38">
         <v>34</v>
@@ -8318,7 +8314,7 @@
         <v>232</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="F48" s="1">
         <v>65</v>
@@ -12024,10 +12020,10 @@
         <v>38</v>
       </c>
       <c r="C254" t="s">
+        <v>294</v>
+      </c>
+      <c r="D254" s="1" t="s">
         <v>295</v>
-      </c>
-      <c r="D254" s="1" t="s">
-        <v>296</v>
       </c>
       <c r="F254" s="1">
         <v>66</v>
@@ -12041,10 +12037,10 @@
         <v>38</v>
       </c>
       <c r="C255" t="s">
+        <v>296</v>
+      </c>
+      <c r="D255" s="1" t="s">
         <v>297</v>
-      </c>
-      <c r="D255" s="1" t="s">
-        <v>298</v>
       </c>
       <c r="F255" s="1">
         <v>67</v>
@@ -12058,13 +12054,13 @@
         <v>43</v>
       </c>
       <c r="C256" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D256" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="E256" s="3" t="s">
         <v>298</v>
-      </c>
-      <c r="E256" s="3" t="s">
-        <v>299</v>
       </c>
       <c r="F256" s="1">
         <v>67</v>
@@ -12078,10 +12074,10 @@
         <v>35</v>
       </c>
       <c r="C257" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D257" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="F257" s="1">
         <v>68</v>
@@ -12095,10 +12091,10 @@
         <v>38</v>
       </c>
       <c r="C258" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D258" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="F258" s="1">
         <v>69</v>
@@ -12112,10 +12108,10 @@
         <v>38</v>
       </c>
       <c r="C259" t="s">
+        <v>301</v>
+      </c>
+      <c r="D259" s="1" t="s">
         <v>302</v>
-      </c>
-      <c r="D259" s="1" t="s">
-        <v>303</v>
       </c>
       <c r="F259" s="1">
         <v>70</v>
@@ -12129,10 +12125,10 @@
         <v>38</v>
       </c>
       <c r="C260" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D260" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F260" s="1">
         <v>71</v>
@@ -14529,10 +14525,10 @@
         <v>42</v>
       </c>
       <c r="D393" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E393" s="3" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="F393" s="1">
         <v>55</v>
@@ -14549,10 +14545,10 @@
         <v>42</v>
       </c>
       <c r="D394" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E394" s="3" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F394" s="1">
         <v>55</v>
@@ -14569,10 +14565,10 @@
         <v>42</v>
       </c>
       <c r="D395" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E395" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="F395" s="1">
         <v>55</v>
@@ -14609,10 +14605,10 @@
         <v>42</v>
       </c>
       <c r="D397" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="E397" s="3" t="s">
         <v>290</v>
-      </c>
-      <c r="E397" s="3" t="s">
-        <v>291</v>
       </c>
       <c r="F397" s="1">
         <v>55</v>
@@ -14629,10 +14625,10 @@
         <v>42</v>
       </c>
       <c r="D398" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="E398" s="3" t="s">
         <v>292</v>
-      </c>
-      <c r="E398" s="3" t="s">
-        <v>293</v>
       </c>
       <c r="F398" s="1">
         <v>55</v>
@@ -14668,14 +14664,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
     </row>
     <row r="2" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
@@ -15827,14 +15823,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="22" t="s">
         <v>73</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="24"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="23"/>
     </row>
     <row r="2" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
@@ -17462,14 +17458,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="22" t="s">
         <v>107</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="24"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="23"/>
     </row>
     <row r="2" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
@@ -18685,14 +18681,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="22" t="s">
         <v>131</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="24"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="23"/>
     </row>
     <row r="2" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
@@ -19865,26 +19861,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="cbd820e2-9c8a-4c01-9a9c-6b4c26777899">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="51aa521f-7cbd-47c5-afee-4a8147a04eed" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100EFCF9BE3DDC69D46817A851BEC5550B1" ma:contentTypeVersion="17" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="254d2fc45a10493323dcacd51be5aaf4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="cbd820e2-9c8a-4c01-9a9c-6b4c26777899" xmlns:ns3="51aa521f-7cbd-47c5-afee-4a8147a04eed" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="003ab9e0b5c5bed7880e662758cd0922" ns2:_="" ns3:_="">
     <xsd:import namespace="cbd820e2-9c8a-4c01-9a9c-6b4c26777899"/>
@@ -20133,32 +20109,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{234FD0E2-0AEF-428D-92BF-35044BB2AB06}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7D755283-77AF-467A-8C74-DC8595DDCA72}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="51aa521f-7cbd-47c5-afee-4a8147a04eed"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="cbd820e2-9c8a-4c01-9a9c-6b4c26777899"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="cbd820e2-9c8a-4c01-9a9c-6b4c26777899">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="51aa521f-7cbd-47c5-afee-4a8147a04eed" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{643D8826-8392-4BEE-9D5B-BD3352057639}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -20175,4 +20146,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{234FD0E2-0AEF-428D-92BF-35044BB2AB06}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7D755283-77AF-467A-8C74-DC8595DDCA72}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="51aa521f-7cbd-47c5-afee-4a8147a04eed"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="cbd820e2-9c8a-4c01-9a9c-6b4c26777899"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>